<commit_message>
update to new "Excel data reader" to avoid 255 maximium characters limitation.
</commit_message>
<xml_diff>
--- a/parser_resources_excel/webapp_resx.xlsx
+++ b/parser_resources_excel/webapp_resx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quan\Documents\project_2023\parser\parser_resources_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3706D0-D74B-4CD7-8371-ADB5895F2E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20BA2C6-C567-4D39-8FA4-0E33123693FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="616">
   <si>
     <t>Id</t>
   </si>
@@ -1868,9 +1868,6 @@
   </si>
   <si>
     <t>Dosi macinate negli ultimi 10 giorni</t>
-  </si>
-  <si>
-    <t>Registrando questo macinacaffè, si dichiare di eserne il proprietario oppure di avere l'autorizzazione del proprietario di accedere alle informazioni del macinacaffè attraverso l'APP, in accordo con i termini di servizio e i relativi aggiornamenti, acQWERTYUI</t>
   </si>
 </sst>
 </file>
@@ -1911,7 +1908,20 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1925,12 +1935,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="translate_mapping" displayName="translate_mapping" ref="A1:C340" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="translate_mapping" displayName="translate_mapping" ref="A1:C340" totalsRowShown="0" dataDxfId="0">
   <autoFilter ref="A1:C340" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="en"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="it"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="en" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="it" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2223,8 +2233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B60" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2991,7 +3001,7 @@
         <v>136</v>
       </c>
       <c r="B70" t="s">
-        <v>616</v>
+        <v>137</v>
       </c>
       <c r="C70" t="s">
         <v>137</v>
@@ -5969,8 +5979,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>